<commit_message>
revert back to before
</commit_message>
<xml_diff>
--- a/SOO_paramInfo/DP1000_room_SwiftVoce_NDBR50_curve1/paramInfo.xlsx
+++ b/SOO_paramInfo/DP1000_room_SwiftVoce_NDBR50_curve1/paramInfo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>parameter</t>
   </si>
@@ -34,12 +34,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>initial</t>
-  </si>
-  <si>
     <t>c1</t>
   </si>
   <si>
@@ -52,24 +46,18 @@
     <t>MPa</t>
   </si>
   <si>
-    <t>yielding</t>
-  </si>
-  <si>
     <t>c2</t>
   </si>
   <si>
     <t>1e-4</t>
   </si>
   <si>
-    <t>e0</t>
+    <t>ε₀</t>
   </si>
   <si>
     <t>dimensionless</t>
   </si>
   <si>
-    <t>hardening</t>
-  </si>
-  <si>
     <t>c3</t>
   </si>
   <si>
@@ -82,19 +70,19 @@
     <t>c4</t>
   </si>
   <si>
-    <t>sigma_y</t>
+    <t>σᵧ</t>
   </si>
   <si>
     <t>c5</t>
   </si>
   <si>
-    <t>sigma_sat</t>
+    <t>Q</t>
   </si>
   <si>
     <t>c6</t>
   </si>
   <si>
-    <t>b</t>
+    <t>β</t>
   </si>
   <si>
     <t>c7</t>
@@ -108,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,12 +107,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -156,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -182,9 +164,6 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -193,9 +172,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,22 +481,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="36.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
@@ -542,12 +518,8 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -559,7 +531,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -568,20 +540,16 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -593,7 +561,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -602,20 +570,16 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -627,7 +591,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -636,20 +600,16 @@
         <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -661,7 +621,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
@@ -670,20 +630,16 @@
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -695,7 +651,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5">
         <v>1</v>
@@ -704,20 +660,16 @@
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -729,7 +681,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -738,20 +690,16 @@
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -763,7 +711,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -772,20 +720,16 @@
         <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -803,7 +747,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="9"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -821,7 +765,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -839,7 +783,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -857,7 +801,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -875,7 +819,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -893,7 +837,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -911,7 +855,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -929,7 +873,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -947,7 +891,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -965,7 +909,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="9"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -983,7 +927,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -995,13 +939,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="6"/>
-      <c r="B20" s="10"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="8"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="9"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>

</xml_diff>